<commit_message>
:bug:Fixed dividend tax credit bug, for provincial, federal keeps the same but never goes wrong...interesting
</commit_message>
<xml_diff>
--- a/Formulars/TaxPro/Alberta/iOS app (excel formula) - AB.xlsx
+++ b/Formulars/TaxPro/Alberta/iOS app (excel formula) - AB.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William.Chong\Desktop\Will\Letter\TaxPro\Base Formula - 2016 for 2017\Alberta\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9132"/>
+    <workbookView xWindow="7680" yWindow="960" windowWidth="24000" windowHeight="13600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RRSP (Deduction)" sheetId="1" r:id="rId1"/>
@@ -18,8 +13,11 @@
     <sheet name="Foreign Investment Inc" sheetId="24" r:id="rId4"/>
     <sheet name="Old Age Security Pension" sheetId="27" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1"/>
+  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -468,7 +466,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,7 +657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +692,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -871,7 +869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -881,24 +879,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
@@ -914,7 +912,7 @@
       <c r="M1" s="47"/>
       <c r="N1" s="47"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -929,7 +927,7 @@
       <c r="M2" s="47"/>
       <c r="N2" s="47"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -944,7 +942,7 @@
       <c r="M3" s="47"/>
       <c r="N3" s="47"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -962,7 +960,7 @@
       <c r="M4" s="47"/>
       <c r="N4" s="47"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
@@ -974,7 +972,7 @@
       <c r="M5" s="47"/>
       <c r="N5" s="47"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
@@ -992,7 +990,7 @@
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1011,7 @@
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1035,7 @@
       <c r="S8" s="52"/>
       <c r="T8" s="52"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="E9" s="47"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
@@ -1055,11 +1053,11 @@
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="H11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1068,19 +1066,19 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="D13" s="4"/>
       <c r="H13" s="82"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="D14" s="4"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="91" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1091,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="21"/>
       <c r="B18" s="91" t="s">
         <v>20</v>
@@ -1106,7 +1104,7 @@
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1123,7 @@
       <c r="H19" s="92"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="21" t="s">
         <v>10</v>
       </c>
@@ -1145,7 +1143,7 @@
       <c r="H20" s="66"/>
       <c r="I20" s="21"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="21" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1163,7 @@
       <c r="H21" s="66"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="21" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1183,7 @@
       <c r="H22" s="66"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="21"/>
       <c r="B23" s="27">
         <f>C22</f>
@@ -1201,7 +1199,7 @@
       <c r="H23" s="66"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="91"/>
@@ -1212,7 +1210,7 @@
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="21" t="s">
         <v>35</v>
       </c>
@@ -1227,7 +1225,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -1238,7 +1236,7 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="91" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1249,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="32" t="s">
         <v>90</v>
       </c>
@@ -1266,7 +1264,7 @@
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="21" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1281,7 @@
       <c r="H29" s="66"/>
       <c r="I29" s="21"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="21" t="s">
         <v>10</v>
       </c>
@@ -1303,7 +1301,7 @@
       <c r="H30" s="66"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="21" t="s">
         <v>10</v>
       </c>
@@ -1323,7 +1321,7 @@
       <c r="H31" s="66"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="21" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1341,7 @@
       <c r="H32" s="66"/>
       <c r="I32" s="21"/>
     </row>
-    <row r="33" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="15">
       <c r="A33" s="21"/>
       <c r="B33" s="27">
         <f>C32</f>
@@ -1359,7 +1357,7 @@
       <c r="H33" s="66"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="91"/>
@@ -1370,7 +1368,7 @@
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
     </row>
-    <row r="35" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="15">
       <c r="A35" s="21" t="s">
         <v>32</v>
       </c>
@@ -1389,7 +1387,7 @@
       <c r="L35" s="4"/>
       <c r="N35" s="4"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14">
       <c r="A36" s="21"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
@@ -1402,7 +1400,7 @@
       <c r="H36" s="20"/>
       <c r="I36" s="21"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14">
       <c r="A37" s="21"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
@@ -1413,7 +1411,7 @@
       <c r="H37" s="20"/>
       <c r="I37" s="21"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14">
       <c r="A38" s="68" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1424,7 @@
       <c r="H38" s="53"/>
       <c r="I38" s="21"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14">
       <c r="B39" s="11"/>
       <c r="C39" t="s">
         <v>13</v>
@@ -1435,7 +1433,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="13"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1450,7 @@
       <c r="K41" s="51"/>
       <c r="L41" s="51"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14">
       <c r="B42" s="37">
         <f>-IF((B12&gt;=B25),IF((B12-B4)&gt;=B25,0,IF(((B12-B4)&lt;B25),((B25-(B12-B4))*D19))),IF(B12&lt;B25,B4*D19))</f>
         <v>0</v>
@@ -1466,7 +1464,7 @@
       <c r="K42" s="51"/>
       <c r="L42" s="51"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14">
       <c r="B43" s="12">
         <f>IF(AND(B12&gt;=B29,B12&lt;=C29),B4*D29,IF(AND(B12&gt;B30,B12&lt;=C30),IF((B12-B30)&gt;B4,B4*D30,((B12-B30)*D30)+((B4-(B12-B30))*D29)),IF(AND(B12&gt;B31,B12&lt;=C31),IF((B12-B31)&gt;B4,B4*D31,IF((B12-B30)&gt;B4,(((B12-B31)*D31)+((B4-(B12-B31))*D30)),(((B12-B31)*D31))+((B31-B30)*D30)+((B4-(B12-B30))*D29))),IF(AND(B12&gt;B32,B12&lt;=C32),IF((B12-B32)&gt;B4,B4*D32,IF((B12-B31)&gt;B4,((B12-B32)*D32)+((B4-(B12-B32))*D31),IF((B12-B30)&gt;B4,((B12-B32)*D32)+((B32-B31)*D31)+((B4-(B12-B31))*D30),((B12-B32)*D32)+((B32-B31)*D31)+((B31-B30)*D30)+((B4-(B12-B30))*D29)))),IF(B12&gt;B33,IF((B12-B33)&gt;B4,B4*D33,IF((B12-B32)&gt;B4,((B12-B33)*D33)+((B4-(B12-B33))*D32),IF((B12-B31)&gt;B4,((B12-B33)*D33)+((B33-B32)*D32)+((B4-(B12-B32))*D31),IF((B12-B30)&gt;B4,((B12-B33)*D33)+((B33-B32)*D32)+((B32-B31)*D31)+((B4-(B12-B31))*D30),((B12-B33)*D33)+((B33-B32)*D32)+((B32-B31)*D31)+((B31-B30)*D30)+((B4-(B12-B30))*D29))))))))))</f>
         <v>100</v>
@@ -1480,7 +1478,7 @@
       <c r="K43" s="51"/>
       <c r="L43" s="51"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14">
       <c r="B44" s="38">
         <f>-IF((B12&gt;=B35),IF((B12-B4)&gt;=B35,0,IF(((B12-B4)&lt;B35),((B35-(B12-B4))*D29))),IF(B12&lt;B35,B4*D29))</f>
         <v>-100</v>
@@ -1494,7 +1492,7 @@
       <c r="K44" s="51"/>
       <c r="L44" s="51"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1509,7 +1507,7 @@
       <c r="K45" s="51"/>
       <c r="L45" s="51"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14">
       <c r="G46" s="51"/>
       <c r="H46" s="51"/>
       <c r="I46" s="51"/>
@@ -1517,7 +1515,7 @@
       <c r="K46" s="51"/>
       <c r="L46" s="51"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14">
       <c r="G47" s="51"/>
       <c r="H47" s="51"/>
       <c r="I47" s="51"/>
@@ -1525,7 +1523,7 @@
       <c r="K47" s="51"/>
       <c r="L47" s="51"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14">
       <c r="G48" s="51"/>
       <c r="H48" s="51"/>
       <c r="I48" s="51"/>
@@ -1533,7 +1531,7 @@
       <c r="K48" s="51"/>
       <c r="L48" s="51"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49" s="19" t="s">
         <v>36</v>
       </c>
@@ -1545,7 +1543,7 @@
       <c r="K49" s="51"/>
       <c r="L49" s="51"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -1554,7 +1552,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -1563,16 +1561,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="B52" s="13">
         <f>SUM(B50:B51)</f>
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="B53" s="15"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64" s="3"/>
     </row>
   </sheetData>
@@ -1582,7 +1580,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1590,34 +1593,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="13" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1637,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1651,7 +1654,7 @@
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1671,7 +1674,7 @@
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="12"/>
@@ -1685,7 +1688,7 @@
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -1699,7 +1702,7 @@
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1716,7 +1719,7 @@
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1736,7 +1739,7 @@
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -1750,7 +1753,7 @@
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="E10" s="21"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
@@ -1764,7 +1767,7 @@
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -1778,7 +1781,7 @@
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1786,13 +1789,13 @@
         <v>139000</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="12"/>
       <c r="I14" s="21"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1801,7 +1804,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1810,7 +1813,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14">
       <c r="B17" s="91" t="s">
         <v>20</v>
       </c>
@@ -1821,7 +1824,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1847,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1868,7 +1871,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1892,7 +1895,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1916,7 +1919,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15">
       <c r="B22" s="27">
         <f>C21</f>
         <v>200000</v>
@@ -1934,7 +1937,7 @@
       <c r="L22" s="5"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14">
       <c r="B23" s="21"/>
       <c r="C23" s="91"/>
       <c r="D23" s="21"/>
@@ -1943,7 +1946,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1957,14 +1960,14 @@
       <c r="H24" s="12"/>
       <c r="I24" s="21"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14">
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="12"/>
       <c r="I25" s="21"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14">
       <c r="A27" s="10" t="s">
         <v>90</v>
       </c>
@@ -1989,7 +1992,7 @@
       <c r="J27" s="10"/>
       <c r="K27" s="25"/>
     </row>
-    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2006,7 +2009,7 @@
       <c r="I28" s="27"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2028,7 +2031,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2051,7 +2054,7 @@
       <c r="L30" s="13"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2074,7 +2077,7 @@
       <c r="L31" s="13"/>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15">
       <c r="B32" s="27">
         <f>C31</f>
         <v>300000</v>
@@ -2091,7 +2094,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="13"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17">
       <c r="B33" s="21"/>
       <c r="C33" s="91"/>
       <c r="D33" s="21"/>
@@ -2103,7 +2106,7 @@
       <c r="K33" s="16"/>
       <c r="L33" s="26"/>
     </row>
-    <row r="34" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2120,7 +2123,7 @@
       <c r="K34" s="16"/>
       <c r="L34" s="26"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" t="s">
@@ -2132,7 +2135,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="21"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -2142,7 +2145,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17">
       <c r="B37" s="11"/>
       <c r="C37" t="s">
         <v>13</v>
@@ -2152,14 +2155,14 @@
       <c r="K37" s="4"/>
       <c r="L37" s="16"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17">
       <c r="H38" s="36"/>
       <c r="I38" s="18"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="16"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2174,7 +2177,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="16"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17">
       <c r="B40" s="37">
         <f>-IF(B12&gt;=B24,0,IF(B12&lt;B24,IF((B12+B4)&gt;B24,(B24-B12)*D18,B4*D18)))</f>
         <v>0</v>
@@ -2186,7 +2189,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="16"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17">
       <c r="B41" s="12">
         <f>IF(AND((B4+B12)&gt;=B28,(B4+B12)&lt;=C28),B4*D28,IF(AND((B4+B12)&gt;B29,(B4+B12)&lt;=C29),IF((B4+B12-B29)&gt;B4,B4*D29,((B4+B12-B29)*D29)+((B4-(B4+B12-B29))*D28)),IF(AND((B4+B12)&gt;B30,(B4+B12)&lt;=C30),IF((B4+B12-B30)&gt;B4,B4*D30,IF((B4+B12-B29)&gt;B4,(((B4+B12-B30)*D30)+((B4-(B4+B12-B30))*D29)),((B4+B12-B30)*D30)+((C29-B29)*D29)+((B4-(B4+B12-B29))*D28))),IF(AND((B4+B12)&gt;B31,(B4+B12)&lt;=C31),IF((B4+B12-B31)&gt;B4,B4*D31,IF((B4+B12-B30)&gt;B4,(((B4+B12-B31)*D31)+((B4-(B4+B12-B31))*D30)),IF((B4+B12-B29)&gt;B4,(((B4+B12-B31)*D31)+((C30-B30)*D30)+((B4-(B4+B12-B30))*D29)),((B4+B12-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B4-(B4+B12-B29))*D28)))),IF((B4+B12)&gt;B32,IF((B4+B12-B32)&gt;B4,B4*D32,IF((B4+B12-B31)&gt;B4,(((B4+B12-B32)*D32)+((B4-(B4+B12-B32))*D31)),IF((B4+B12-B30)&gt;B4,(((B4+B12-B32)*D32)+((C31-B31)*D31)+((B4-(B4+B12-B31))*D30)),IF((B4+B12-B29)&gt;B4,(((B4+B12-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((B4-(B4+B12-B30))*D29)),((B4+B12-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B4-(B4+B12-B29))*D28))))))))))</f>
         <v>120</v>
@@ -2195,7 +2198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17">
       <c r="B42" s="38">
         <f>-IF(B12&gt;=B34,0,IF(B12&lt;B34,IF((B12+B4)&gt;B34,(B34-B12)*D28,B4*D28)))</f>
         <v>0</v>
@@ -2204,7 +2207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17">
       <c r="A43" s="10" t="s">
         <v>21</v>
       </c>
@@ -2221,7 +2224,7 @@
       <c r="L43" s="48"/>
       <c r="M43" s="47"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17">
       <c r="E44" s="18"/>
       <c r="F44" s="49"/>
       <c r="G44" s="47"/>
@@ -2233,7 +2236,7 @@
       <c r="M44" s="47"/>
       <c r="Q44" s="15"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17">
       <c r="B45" s="13"/>
       <c r="F45" s="47"/>
       <c r="G45" s="47"/>
@@ -2244,7 +2247,7 @@
       <c r="L45" s="47"/>
       <c r="M45" s="47"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17">
       <c r="A46" s="19" t="s">
         <v>36</v>
       </c>
@@ -2258,7 +2261,7 @@
       <c r="L46" s="47"/>
       <c r="M46" s="47"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -2275,7 +2278,7 @@
       <c r="L47" s="47"/>
       <c r="M47" s="47"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -2292,7 +2295,7 @@
       <c r="L48" s="47"/>
       <c r="M48" s="47"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13">
       <c r="B49" s="13">
         <f>SUM(B47:B48)</f>
         <v>380</v>
@@ -2306,7 +2309,7 @@
       <c r="L49" s="47"/>
       <c r="M49" s="47"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13">
       <c r="B50" s="13"/>
       <c r="F50" s="47"/>
       <c r="G50" s="47"/>
@@ -2317,7 +2320,7 @@
       <c r="L50" s="47"/>
       <c r="M50" s="47"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13">
       <c r="B51" s="13"/>
       <c r="F51" s="47"/>
       <c r="G51" s="47"/>
@@ -2328,7 +2331,7 @@
       <c r="L51" s="47"/>
       <c r="M51" s="47"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13">
       <c r="B52" s="13"/>
       <c r="F52" s="47"/>
       <c r="G52" s="47"/>
@@ -2339,7 +2342,7 @@
       <c r="L52" s="47"/>
       <c r="M52" s="47"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13">
       <c r="B53" s="13"/>
       <c r="F53" s="47"/>
       <c r="G53" s="47"/>
@@ -2350,7 +2353,7 @@
       <c r="L53" s="47"/>
       <c r="M53" s="47"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:13">
       <c r="B54" s="15"/>
       <c r="F54" s="47"/>
       <c r="G54" s="47"/>
@@ -2361,7 +2364,7 @@
       <c r="L54" s="47"/>
       <c r="M54" s="47"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:13">
       <c r="F55" s="47"/>
       <c r="G55" s="47"/>
       <c r="H55" s="46"/>
@@ -2371,7 +2374,7 @@
       <c r="L55" s="47"/>
       <c r="M55" s="47"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:13">
       <c r="F56" s="47"/>
       <c r="G56" s="47"/>
       <c r="H56" s="46"/>
@@ -2381,7 +2384,7 @@
       <c r="L56" s="47"/>
       <c r="M56" s="47"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:13">
       <c r="F57" s="47"/>
       <c r="G57" s="47"/>
       <c r="H57" s="46"/>
@@ -2391,16 +2394,21 @@
       <c r="L57" s="47"/>
       <c r="M57" s="47"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13">
       <c r="H58" s="12"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:13">
       <c r="H60" s="40"/>
       <c r="M60" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2408,28 +2416,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="13" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
@@ -2444,7 +2452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2458,7 +2466,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -2470,7 +2478,7 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="E4" t="s">
         <v>55</v>
       </c>
@@ -2485,12 +2493,12 @@
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="56">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="E5" t="s">
         <v>56</v>
@@ -2506,7 +2514,7 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="28">
       <c r="A6" s="28" t="s">
         <v>39</v>
       </c>
@@ -2525,12 +2533,12 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -2542,7 +2550,7 @@
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="A8" s="28"/>
       <c r="E8" s="47"/>
       <c r="F8" s="47"/>
@@ -2555,7 +2563,7 @@
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="A9" s="30" t="s">
         <v>59</v>
       </c>
@@ -2571,7 +2579,7 @@
       <c r="M9" s="47"/>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="A10" s="28" t="s">
         <v>57</v>
       </c>
@@ -2590,12 +2598,12 @@
       <c r="M10" s="80"/>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14">
       <c r="A11" s="28" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="1">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="47"/>
@@ -2609,7 +2617,7 @@
       <c r="M11" s="80"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="21" customFormat="1">
       <c r="A12" s="57"/>
       <c r="B12"/>
       <c r="D12" s="47"/>
@@ -2623,7 +2631,7 @@
       <c r="L12" s="80"/>
       <c r="M12" s="80"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2639,7 +2647,7 @@
       <c r="M13" s="47"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2658,7 +2666,7 @@
       <c r="M14" s="47"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14">
       <c r="D15" s="47"/>
       <c r="E15" s="47"/>
       <c r="F15" s="47"/>
@@ -2671,7 +2679,7 @@
       <c r="M15" s="47"/>
       <c r="N15" s="21"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14">
       <c r="D16" s="47"/>
       <c r="E16" s="47"/>
       <c r="F16" s="78"/>
@@ -2684,7 +2692,7 @@
       <c r="M16" s="47"/>
       <c r="N16" s="21"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14">
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
@@ -2697,23 +2705,23 @@
       <c r="M17" s="47"/>
       <c r="N17" s="21"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1">
-        <v>139000</v>
+        <v>90000</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -2723,7 +2731,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="21"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14">
       <c r="B21" s="91" t="s">
         <v>20</v>
       </c>
@@ -2735,7 +2743,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2755,7 +2763,7 @@
       <c r="I22" s="21"/>
       <c r="N22" s="6"/>
     </row>
-    <row r="23" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2776,7 +2784,7 @@
       <c r="I23" s="21"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2797,7 +2805,7 @@
       <c r="I24" s="21"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2818,7 +2826,7 @@
       <c r="I25" s="21"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15">
       <c r="B26" s="27">
         <f>C25</f>
         <v>200000</v>
@@ -2834,7 +2842,7 @@
       <c r="I26" s="21"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14">
       <c r="B27" s="21"/>
       <c r="C27" s="91"/>
       <c r="D27" s="21"/>
@@ -2844,7 +2852,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2859,14 +2867,14 @@
       <c r="H28" s="12"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14">
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="12"/>
       <c r="I29" s="21"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -2876,7 +2884,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14">
       <c r="A31" s="10" t="s">
         <v>90</v>
       </c>
@@ -2893,7 +2901,7 @@
       <c r="J31" s="32"/>
       <c r="K31" s="70"/>
     </row>
-    <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2912,7 +2920,7 @@
       <c r="J32" s="66"/>
       <c r="K32" s="21"/>
     </row>
-    <row r="33" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2935,7 +2943,7 @@
       <c r="K33" s="53"/>
       <c r="L33" s="15"/>
     </row>
-    <row r="34" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2959,7 +2967,7 @@
       <c r="L34" s="13"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2983,7 +2991,7 @@
       <c r="L35" s="13"/>
       <c r="N35" s="4"/>
     </row>
-    <row r="36" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="15">
       <c r="B36" s="27">
         <f>C35</f>
         <v>300000</v>
@@ -3001,7 +3009,7 @@
       <c r="K36" s="52"/>
       <c r="L36" s="13"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17">
       <c r="B37" s="21"/>
       <c r="C37" s="91"/>
       <c r="D37" s="21"/>
@@ -3014,7 +3022,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="26"/>
     </row>
-    <row r="38" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="15">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -3029,7 +3037,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="26"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" t="s">
@@ -3042,7 +3050,7 @@
       <c r="J39" s="21"/>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="E40" s="13"/>
@@ -3052,7 +3060,7 @@
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -3070,7 +3078,7 @@
       <c r="K41" s="21"/>
       <c r="Q41" s="18"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17">
       <c r="B42" s="37"/>
       <c r="C42" s="69" t="s">
         <v>86</v>
@@ -3093,7 +3101,7 @@
       </c>
       <c r="Q42" s="18"/>
     </row>
-    <row r="43" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15">
       <c r="A43" s="28" t="s">
         <v>87</v>
       </c>
@@ -3118,14 +3126,14 @@
       </c>
       <c r="J43" s="12">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=F43,($B$18+$B$5+$B$67)&lt;G43),($B$18+$B$5+$B$67-F43)*H43,0)</f>
-        <v>0</v>
+        <v>9800</v>
       </c>
       <c r="K43" s="53">
         <f t="shared" ref="K43:K47" ca="1" si="1">(IF(J43=0,0,I43+J43))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="15">
       <c r="A44" s="28" t="s">
         <v>41</v>
       </c>
@@ -3152,14 +3160,14 @@
       </c>
       <c r="J44" s="12">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=F44,($B$18+$B$5+$B$67)&lt;G44),($B$18+$B$5+$B$67-F44)*H44,0)</f>
-        <v>1920</v>
+        <v>0</v>
       </c>
       <c r="K44" s="53">
         <f t="shared" ca="1" si="1"/>
-        <v>14420</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="15">
       <c r="A45" s="28" t="s">
         <v>40</v>
       </c>
@@ -3194,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15">
       <c r="A46" s="28" t="s">
         <v>42</v>
       </c>
@@ -3229,13 +3237,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15">
       <c r="A47" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="42">
         <f>IF(B6="non-canadian corporation",B5,0)</f>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="30"/>
@@ -3260,10 +3268,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17">
       <c r="B48" s="18">
         <f>SUM(B45:B47)</f>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="D48" s="21"/>
       <c r="F48" s="13"/>
@@ -3273,10 +3281,10 @@
       <c r="J48" s="21"/>
       <c r="K48" s="53">
         <f ca="1">SUM(K43:K47)</f>
-        <v>14420</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="B49" s="18"/>
       <c r="D49" s="21"/>
       <c r="F49" s="13"/>
@@ -3297,7 +3305,7 @@
         <v>1845.1000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17">
       <c r="A50" s="19" t="s">
         <v>37</v>
       </c>
@@ -3312,11 +3320,11 @@
       <c r="J50" s="21"/>
       <c r="K50" s="13">
         <f ca="1">IF((K48-K49)&lt;=0,0,K48-K49)</f>
-        <v>12574.9</v>
+        <v>7954.9</v>
       </c>
       <c r="Q50" s="18"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -3341,7 +3349,7 @@
       </c>
       <c r="Q51" s="18"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -3358,11 +3366,11 @@
       <c r="J52" s="21"/>
       <c r="K52" s="12">
         <f ca="1">K50-K51</f>
-        <v>12574.9</v>
+        <v>7954.9</v>
       </c>
       <c r="Q52" s="18"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17">
       <c r="B53" s="37">
         <f ca="1">SUM(B51:B52)</f>
         <v>0</v>
@@ -3377,11 +3385,11 @@
       <c r="J53" s="21"/>
       <c r="K53" s="75">
         <f ca="1">MIN(B99,K52)</f>
-        <v>0</v>
+        <v>3.3728571428571286</v>
       </c>
       <c r="Q53" s="18"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17">
       <c r="B54" s="37"/>
       <c r="C54" s="4"/>
       <c r="D54" s="21"/>
@@ -3390,11 +3398,11 @@
       <c r="J54" s="21"/>
       <c r="K54" s="12">
         <f ca="1">K52-K53</f>
-        <v>12574.9</v>
+        <v>7951.5271428571423</v>
       </c>
       <c r="Q54" s="18"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17">
       <c r="A55" s="19" t="s">
         <v>93</v>
       </c>
@@ -3410,7 +3418,7 @@
       <c r="K55" s="21"/>
       <c r="Q55" s="18"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3427,7 +3435,7 @@
       <c r="K56" s="21"/>
       <c r="Q56" s="18"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -3444,7 +3452,7 @@
       <c r="K57" s="21"/>
       <c r="Q57" s="18"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17">
       <c r="B58" s="37">
         <f ca="1">SUM(B56:B57)</f>
         <v>0</v>
@@ -3456,7 +3464,7 @@
       <c r="K58" s="21"/>
       <c r="Q58" s="18"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17">
       <c r="B59" s="37"/>
       <c r="C59" s="4"/>
       <c r="D59" s="21"/>
@@ -3465,7 +3473,7 @@
       <c r="K59" s="21"/>
       <c r="Q59" s="18"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17">
       <c r="A60" s="3" t="s">
         <v>50</v>
       </c>
@@ -3477,7 +3485,7 @@
       <c r="K60" s="21"/>
       <c r="Q60" s="18"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17">
       <c r="B61" s="37"/>
       <c r="C61" s="4"/>
       <c r="I61" s="47"/>
@@ -3485,7 +3493,7 @@
       <c r="K61" s="21"/>
       <c r="Q61" s="18"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17">
       <c r="A62" s="19" t="s">
         <v>51</v>
       </c>
@@ -3497,13 +3505,13 @@
       <c r="K62" s="21"/>
       <c r="Q62" s="18"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>71</v>
       </c>
       <c r="B63" s="37">
         <f>$B$5</f>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="C63" s="60" t="s">
         <v>28</v>
@@ -3526,13 +3534,13 @@
       <c r="K63" s="21"/>
       <c r="Q63" s="18"/>
     </row>
-    <row r="64" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="15">
       <c r="A64" t="s">
         <v>72</v>
       </c>
       <c r="B64" s="37">
         <f>IF($B$10="US",-IF(($B$11/$B$5)&gt;15%,$B$11-($B$5*15%),0),0)</f>
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="C64" s="60" t="s">
         <v>29</v>
@@ -3565,7 +3573,7 @@
       <c r="K64" s="21"/>
       <c r="Q64" s="18"/>
     </row>
-    <row r="65" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="15">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -3604,7 +3612,7 @@
       <c r="K65" s="21"/>
       <c r="Q65" s="18"/>
     </row>
-    <row r="66" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="15">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -3634,16 +3642,16 @@
       </c>
       <c r="I66" s="12">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=E66,($B$18+$B$5+$B$67)&lt;F66),($B$18+$B$5+$B$67-E66)*G66,0)</f>
-        <v>0</v>
+        <v>1933.6200000000001</v>
       </c>
       <c r="J66" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>18008.524999999998</v>
       </c>
       <c r="K66" s="21"/>
       <c r="Q66" s="18"/>
     </row>
-    <row r="67" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="15">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -3675,22 +3683,22 @@
       </c>
       <c r="I67" s="12">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=E67,($B$18+$B$5+$B$67)&lt;F67),($B$18+$B$5+$B$67-E67)*G67,0)</f>
-        <v>177.48</v>
+        <v>0</v>
       </c>
       <c r="J67" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>29206.884999999998</v>
+        <v>0</v>
       </c>
       <c r="K67" s="21"/>
       <c r="Q67" s="18"/>
     </row>
-    <row r="68" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="15">
       <c r="A68" t="s">
         <v>53</v>
       </c>
       <c r="B68" s="37">
         <f ca="1">B63+B64+B67</f>
-        <v>2000</v>
+        <v>7200</v>
       </c>
       <c r="C68" s="60" t="s">
         <v>81</v>
@@ -3718,7 +3726,7 @@
       <c r="K68" s="21"/>
       <c r="Q68" s="18"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17">
       <c r="B69" s="37"/>
       <c r="C69" s="4"/>
       <c r="E69" s="13"/>
@@ -3728,18 +3736,18 @@
       <c r="I69" s="47"/>
       <c r="J69" s="12">
         <f ca="1">SUM(J64:J68)</f>
-        <v>29206.884999999998</v>
+        <v>18008.524999999998</v>
       </c>
       <c r="K69" s="21"/>
       <c r="Q69" s="18"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>6</v>
       </c>
       <c r="B70" s="39">
         <f>$B$5+$B$18</f>
-        <v>141000</v>
+        <v>98000</v>
       </c>
       <c r="C70" s="60" t="s">
         <v>28</v>
@@ -3762,7 +3770,7 @@
       <c r="K70" s="21"/>
       <c r="Q70" s="18"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -3775,12 +3783,12 @@
       <c r="I71" s="47"/>
       <c r="J71" s="13">
         <f ca="1">IF((J69-J70)&lt;=0,0,J69-J70)</f>
-        <v>27485.785</v>
+        <v>16287.424999999997</v>
       </c>
       <c r="K71" s="21"/>
       <c r="Q71" s="18"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3795,7 +3803,7 @@
       <c r="K72" s="21"/>
       <c r="Q72" s="18"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -3813,13 +3821,13 @@
       <c r="K73" s="21"/>
       <c r="Q73" s="18"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="37">
         <f ca="1">B70+B73</f>
-        <v>141000</v>
+        <v>98000</v>
       </c>
       <c r="C74" s="60" t="s">
         <v>82</v>
@@ -3829,7 +3837,7 @@
       <c r="K74" s="21"/>
       <c r="Q74" s="18"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17">
       <c r="B75" s="37"/>
       <c r="C75" s="4"/>
       <c r="I75" s="47"/>
@@ -3837,13 +3845,13 @@
       <c r="K75" s="21"/>
       <c r="Q75" s="18"/>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>54</v>
       </c>
       <c r="B76" s="59">
         <f ca="1">B68/B74</f>
-        <v>1.4184397163120567E-2</v>
+        <v>7.3469387755102047E-2</v>
       </c>
       <c r="C76" s="4"/>
       <c r="I76" s="47"/>
@@ -3851,7 +3859,7 @@
       <c r="K76" s="21"/>
       <c r="Q76" s="18"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17">
       <c r="B77" s="37"/>
       <c r="C77" s="4"/>
       <c r="I77" s="47"/>
@@ -3859,13 +3867,13 @@
       <c r="K77" s="21"/>
       <c r="Q77" s="18"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>52</v>
       </c>
       <c r="B78" s="37">
         <f ca="1">J71</f>
-        <v>27485.785</v>
+        <v>16287.424999999997</v>
       </c>
       <c r="C78" s="4"/>
       <c r="I78" s="47"/>
@@ -3873,7 +3881,7 @@
       <c r="K78" s="21"/>
       <c r="Q78" s="18"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17">
       <c r="B79" s="37"/>
       <c r="C79" s="4"/>
       <c r="E79" s="65"/>
@@ -3885,13 +3893,13 @@
       <c r="K79" s="21"/>
       <c r="Q79" s="18"/>
     </row>
-    <row r="80" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="15">
       <c r="A80" t="s">
         <v>64</v>
       </c>
       <c r="B80" s="37">
         <f ca="1">B78*B76</f>
-        <v>389.86929078014185</v>
+        <v>1196.6271428571429</v>
       </c>
       <c r="C80" s="60" t="s">
         <v>28</v>
@@ -3904,13 +3912,13 @@
       <c r="K80" s="21"/>
       <c r="Q80" s="18"/>
     </row>
-    <row r="81" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" ht="15">
       <c r="A81" t="s">
         <v>65</v>
       </c>
       <c r="B81" s="37">
         <f>IF(B6="Canadian Corporation",0,MIN($B$11,$B$5*15%))</f>
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="C81" s="60" t="s">
         <v>29</v>
@@ -3923,7 +3931,7 @@
       <c r="K81" s="21"/>
       <c r="Q81" s="18"/>
     </row>
-    <row r="82" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" ht="15">
       <c r="B82" s="37"/>
       <c r="C82" s="4"/>
       <c r="E82" s="5"/>
@@ -3934,13 +3942,13 @@
       <c r="K82" s="21"/>
       <c r="Q82" s="18"/>
     </row>
-    <row r="83" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" ht="15">
       <c r="A83" t="s">
         <v>66</v>
       </c>
       <c r="B83" s="62">
         <f ca="1">MIN(B80,B81)</f>
-        <v>200</v>
+        <v>1196.6271428571429</v>
       </c>
       <c r="C83" s="60" t="s">
         <v>84</v>
@@ -3953,7 +3961,7 @@
       <c r="K83" s="21"/>
       <c r="Q83" s="18"/>
     </row>
-    <row r="84" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="15">
       <c r="B84" s="62"/>
       <c r="C84" s="4"/>
       <c r="E84" s="5"/>
@@ -3965,7 +3973,7 @@
       <c r="K84" s="21"/>
       <c r="Q84" s="18"/>
     </row>
-    <row r="85" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" ht="15">
       <c r="B85" s="62"/>
       <c r="C85" s="4"/>
       <c r="E85" s="13"/>
@@ -3977,7 +3985,7 @@
       <c r="K85" s="21"/>
       <c r="Q85" s="18"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17">
       <c r="A86" s="19" t="s">
         <v>67</v>
       </c>
@@ -3990,13 +3998,13 @@
       <c r="L86" s="19"/>
       <c r="Q86" s="18"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17">
       <c r="A87" t="s">
         <v>53</v>
       </c>
       <c r="B87" s="37">
         <f ca="1">B68</f>
-        <v>2000</v>
+        <v>7200</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="19" t="s">
@@ -4017,13 +4025,13 @@
       <c r="K87" s="53"/>
       <c r="Q87" s="18"/>
     </row>
-    <row r="88" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="15">
       <c r="A88" t="s">
         <v>22</v>
       </c>
       <c r="B88" s="39">
         <f ca="1">B74</f>
-        <v>141000</v>
+        <v>98000</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" t="s">
@@ -4045,22 +4053,22 @@
       </c>
       <c r="I88" s="46">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=E88,($B$18+$B$5+$B$67)&lt;F88),($B$18+$B$5+$B$67-E88)*G88,0)</f>
-        <v>0</v>
+        <v>9800</v>
       </c>
       <c r="J88" s="12">
         <f ca="1">(IF(I88=0,0,H88+I88))</f>
-        <v>0</v>
+        <v>9800</v>
       </c>
       <c r="K88" s="21"/>
       <c r="Q88" s="18"/>
     </row>
-    <row r="89" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" ht="15">
       <c r="A89" t="s">
         <v>54</v>
       </c>
       <c r="B89" s="59">
         <f ca="1">B87/B88</f>
-        <v>1.4184397163120567E-2</v>
+        <v>7.3469387755102047E-2</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" t="s">
@@ -4084,16 +4092,16 @@
       </c>
       <c r="I89" s="46">
         <f ca="1">IF(AND(($B$18+$B$5+$B$67)&gt;=E89,($B$18+$B$5+$B$67)&lt;F89),($B$18+$B$5+$B$67-E89)*G89,0)</f>
-        <v>1920</v>
+        <v>0</v>
       </c>
       <c r="J89" s="12">
         <f t="shared" ref="J89:J92" ca="1" si="6">(IF(I89=0,0,H89+I89))</f>
-        <v>14420</v>
+        <v>0</v>
       </c>
       <c r="K89" s="21"/>
       <c r="Q89" s="18"/>
     </row>
-    <row r="90" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" ht="15">
       <c r="B90" s="37"/>
       <c r="C90" s="4"/>
       <c r="D90" t="s">
@@ -4126,13 +4134,13 @@
       <c r="K90" s="21"/>
       <c r="Q90" s="18"/>
     </row>
-    <row r="91" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" ht="15">
       <c r="A91" t="s">
         <v>68</v>
       </c>
       <c r="B91" s="37">
         <f ca="1">J95</f>
-        <v>12574.9</v>
+        <v>7954.9</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" t="s">
@@ -4165,7 +4173,7 @@
       <c r="K91" s="21"/>
       <c r="Q91" s="18"/>
     </row>
-    <row r="92" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" ht="15">
       <c r="B92" s="37"/>
       <c r="C92" s="4"/>
       <c r="E92" s="5">
@@ -4191,13 +4199,13 @@
       <c r="K92" s="21"/>
       <c r="Q92" s="18"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>64</v>
       </c>
       <c r="B93" s="37">
         <f ca="1">B91*B89</f>
-        <v>178.36737588652483</v>
+        <v>584.44163265306122</v>
       </c>
       <c r="C93" s="60" t="s">
         <v>28</v>
@@ -4209,12 +4217,12 @@
       <c r="I93" s="47"/>
       <c r="J93" s="53">
         <f ca="1">SUM(J88:J92)</f>
-        <v>14420</v>
+        <v>9800</v>
       </c>
       <c r="K93" s="21"/>
       <c r="Q93" s="18"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17">
       <c r="B94" s="37"/>
       <c r="C94" s="60"/>
       <c r="E94" s="13"/>
@@ -4237,13 +4245,13 @@
       <c r="K94" s="21"/>
       <c r="Q94" s="18"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17">
       <c r="A95" t="s">
         <v>65</v>
       </c>
       <c r="B95" s="37">
         <f>B81</f>
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="E95" s="36"/>
       <c r="F95" s="21"/>
@@ -4252,17 +4260,17 @@
       <c r="I95" s="47"/>
       <c r="J95" s="13">
         <f ca="1">IF((J93-J94)&lt;=0,0,J93-J94)</f>
-        <v>12574.9</v>
+        <v>7954.9</v>
       </c>
       <c r="K95" s="21"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17">
       <c r="A96" t="s">
         <v>75</v>
       </c>
       <c r="B96" s="38">
         <f ca="1">-B83</f>
-        <v>-200</v>
+        <v>-1196.6271428571429</v>
       </c>
       <c r="C96" s="60"/>
       <c r="F96" s="39"/>
@@ -4272,10 +4280,10 @@
       <c r="J96" s="49"/>
       <c r="K96" s="21"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12">
       <c r="B97" s="37">
         <f ca="1">SUM(B95:B96)</f>
-        <v>0</v>
+        <v>3.3728571428571286</v>
       </c>
       <c r="C97" s="60" t="s">
         <v>29</v>
@@ -4286,7 +4294,7 @@
       <c r="J97" s="12"/>
       <c r="K97" s="21"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12">
       <c r="B98" s="37"/>
       <c r="C98" s="4"/>
       <c r="H98" s="18"/>
@@ -4295,13 +4303,13 @@
       <c r="K98" s="52"/>
       <c r="L98" s="16"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>69</v>
       </c>
       <c r="B99" s="62">
         <f ca="1">MIN(B93,B97)</f>
-        <v>0</v>
+        <v>3.3728571428571286</v>
       </c>
       <c r="C99" s="60" t="s">
         <v>84</v>
@@ -4311,7 +4319,7 @@
       <c r="K99" s="52"/>
       <c r="L99" s="16"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12">
       <c r="B100" s="37"/>
       <c r="C100" s="4"/>
       <c r="I100" s="47"/>
@@ -4319,7 +4327,7 @@
       <c r="K100" s="52"/>
       <c r="L100" s="16"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>83</v>
       </c>
@@ -4337,7 +4345,7 @@
       <c r="K101" s="52"/>
       <c r="L101" s="16"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12">
       <c r="B102" s="37"/>
       <c r="C102" s="4"/>
       <c r="G102" s="18"/>
@@ -4347,7 +4355,7 @@
       <c r="K102" s="52"/>
       <c r="L102" s="16"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12">
       <c r="A103" s="2" t="s">
         <v>12</v>
       </c>
@@ -4358,7 +4366,7 @@
       <c r="K103" s="48"/>
       <c r="L103" s="16"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12">
       <c r="B104" s="11"/>
       <c r="C104" t="s">
         <v>13</v>
@@ -4370,7 +4378,7 @@
       <c r="K104" s="48"/>
       <c r="L104" s="16"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12">
       <c r="B105" s="37"/>
       <c r="C105" s="4"/>
       <c r="H105" s="46"/>
@@ -4379,13 +4387,13 @@
       <c r="K105" s="47"/>
       <c r="L105" s="16"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>19</v>
       </c>
       <c r="B106" s="37">
         <f ca="1">IF(AND((B5+B67+B18)&gt;=B22,(B5+B67+B18)&lt;=C22),(B5+B67)*D22,IF(AND((B5+B67+B18)&gt;B23,(B5+B67+B18)&lt;=C23),IF((B5+B67+B18-B23)&gt;(B5+B67),(B5+B67)*D23,((B5+B67+B18-B23)*D23)+((B5+B67-(B5+B67+B18-B23))*D22)),IF(AND((B5+B67+B18)&gt;B24,(B5+B67+B18)&lt;=C24),IF((B5+B67+B18-B24)&gt;(B5+B67),(B5+B67)*D24,IF((B5+B67+B18-B23)&gt;(B5+B67),(((B5+B67+B18-B24)*D24)+((B5+B67-(B5+B67+B18-B24))*D23)),((B5+B67+B18-B24)*D24)+((C23-B23)*D23)+((B5+B67-(B5+B67+B18-B23))*D22))),IF(AND((B5+B67+B18)&gt;B25,(B5+B67+B18)&lt;=C25),IF((B5+B67+B18-B25)&gt;(B5+B67),(B5+B67)*D25,IF((B5+B67+B18-B24)&gt;(B5+B67),((B5+B67+B18-B25)*D25)+(((B5+B67-(B5+B67+B18-B25))*D24)),IF((B5+B67+B18-B23)&gt;(B5+B67),(((B5+B67+B18-B25)*D25)+((C24-B24)*D24)+((B5+B67-(B5+B67+B18-B24))*D23)),((B5+B67+B18-B25)*D25)+((C24-B24)*D24)+((C23-B23)*D23)+((B5+B67-(B5+B67+B18-B23))*D22)))),IF((B5+B67+B18)&gt;B26,IF((B5+B67+B18-B26)&gt;(B5+B67),(B5+B67)*D26,IF((B5+B67+B18-B25)&gt;(B5+B67),(((B5+B67+B18-B26)*D26)+((B5+B67-(B5+B67+B18-B26))*D25)),IF((B5+B67+B18-B24)&gt;(B5+B67),(((B5+B67+B18-B26)*D26)+((C25-B25)*D25)+((B5+B67-(B5+B67+B18-B25))*D24)),IF((B5+B67+B18-B23)&gt;(B5+B67),(((B5+B67+B18-B26)*D26)+((C25-B25)*D25)+((C24-B24)*D24)+((B5+B67-(B5+B67+B18-B24))*D23)),((B5+B67+B18-B26)*D26)+((C25-B25)*D25)+((C24-B24)*D24)+((C23-B23)*D23)+((B5+B67-(B5+B67+B18-B23))*D22))))))))))</f>
-        <v>538.36</v>
+        <v>2049.0350000000003</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
@@ -4397,7 +4405,7 @@
       <c r="K106" s="47"/>
       <c r="L106" s="13"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12">
       <c r="B107" s="37">
         <f>-IF(B18&gt;=B28,0,IF(B18&lt;B28,IF((B18+B5+B67)&gt;B28,(B28-B18)*D22,((B5+B67)*D22))))</f>
         <v>0</v>
@@ -4412,7 +4420,7 @@
       <c r="K107" s="48"/>
       <c r="L107" s="16"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12">
       <c r="B108" s="37">
         <f ca="1">-B53</f>
         <v>0</v>
@@ -4427,10 +4435,10 @@
       <c r="K108" s="52"/>
       <c r="L108" s="16"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12">
       <c r="B109" s="37">
         <f ca="1">IF(B83=0,0,-MIN(B83,SUM(B106:B108)))</f>
-        <v>-200</v>
+        <v>-1196.6271428571429</v>
       </c>
       <c r="C109" t="s">
         <v>76</v>
@@ -4442,10 +4450,10 @@
       <c r="K109" s="52"/>
       <c r="L109" s="16"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12">
       <c r="B110" s="37">
         <f ca="1">IF(AND((B5+B67+B18)&gt;=B32,(B5+B67+B18)&lt;=C32),(B5+B67)*D32,IF(AND((B5+B67+B18)&gt;B33,(B5+B67+B18)&lt;=C33),IF((B5+B67+B18-B33)&gt;(B5+B67),(B5+B67)*D33,((B5+B67+B18-B33)*D33)+((B5+B67-(B5+B67+B18-B33))*D32)),IF(AND((B5+B67+B18)&gt;B34,(B5+B67+B18)&lt;=C34),IF((B5+B67+B18-B34)&gt;(B5+B67),(B5+B67)*D34,IF((B5+B67+B18-B33)&gt;(B5+B67),(((B5+B67+B18-B34)*D34)+((B5+B67-(B5+B67+B18-B34))*D33)),((B5+B67+B18-B34)*D34)+((C33-B33)*D33)+((B5+B67-(B5+B67+B18-B33))*D32))),IF(AND((B5+B67+B18)&gt;B35,(B5+B67+B18)&lt;=C35),IF((B5+B67+B18-B35)&gt;(B5+B67),(B5+B67)*D35,IF((B5+B67+B18-B34)&gt;(B5+B67),(((B5+B67+B18-B35)*D35)+((B5+B67-(B5+B67+B18-B35))*D34)),IF((B5+B67+B18-B33)&gt;(B5+B67),(((B5+B67+B18-B35)*D35)+((C34-B34)*D34)+((B5+B67-(B5+B67+B18-B34))*D33)),((B5+B67+B18-B35)*D35)+((C34-B34)*D34)+((C33-B33)*D33)+((B5+B67-(B5+B67+B18-B33))*D32)))),IF((B5+B67+B18)&gt;B36,IF((B5+B67+B18-B36)&gt;(B5+B67),(B5+B67)*D36,IF((B5+B67+B18-B35)&gt;(B5+B67),(((B5+B67+B18-B36)*D36)+((B5+B67-(B5+B67+B18-B36))*D35)),IF((B5+B67+B18-B34)&gt;(B5+B67),(((B5+B67+B18-B36)*D36)+((C35-B35)*D35)+((B5+B67-(B5+B67+B18-B35))*D34)),IF((B5+B67+B18-B33)&gt;(B5+B67),(((B5+B67+B18-B36)*D36)+((C35-B35)*D35)+((C34-B34)*D34)+((B5+B67-(B5+B67+B18-B34))*D33)),((B5+B67+B18-B36)*D36)+((C35-B35)*D35)+((C34-B34)*D34)+((C33-B33)*D33)+((B5+B67-(B5+B67+B18-B33))*D32))))))))))</f>
-        <v>240</v>
+        <v>800</v>
       </c>
       <c r="C110" t="s">
         <v>16</v>
@@ -4456,7 +4464,7 @@
       <c r="J110" s="53"/>
       <c r="K110" s="21"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12">
       <c r="B111" s="37">
         <f>-IF(B18&gt;=B38,0,IF(B18&lt;B38,IF((B18+B5+B67)&gt;B38,(B38-B18)*D32,((B5+B67)*D32))))</f>
         <v>0</v>
@@ -4471,7 +4479,7 @@
       <c r="K111" s="52"/>
       <c r="L111" s="13"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12">
       <c r="B112" s="37">
         <f ca="1">-B58</f>
         <v>0</v>
@@ -4485,10 +4493,10 @@
       <c r="J112" s="21"/>
       <c r="K112" s="21"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17">
       <c r="B113" s="38">
         <f ca="1">IF(B99=0,0,-MIN(B99,SUM(B110,B111,B112)))</f>
-        <v>0</v>
+        <v>-3.3728571428571286</v>
       </c>
       <c r="C113" t="s">
         <v>77</v>
@@ -4500,13 +4508,13 @@
       <c r="K113" s="21"/>
       <c r="L113" s="13"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17">
       <c r="A114" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B114" s="79">
         <f ca="1">SUM(B106:B113)</f>
-        <v>578.36</v>
+        <v>1649.0350000000003</v>
       </c>
       <c r="F114" s="47"/>
       <c r="I114" s="21"/>
@@ -4515,7 +4523,7 @@
       <c r="L114" s="48"/>
       <c r="M114" s="47"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17">
       <c r="E115" s="18"/>
       <c r="F115" s="49"/>
       <c r="K115" s="47"/>
@@ -4523,14 +4531,14 @@
       <c r="M115" s="47"/>
       <c r="Q115" s="15"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17">
       <c r="B116" s="13"/>
       <c r="F116" s="47"/>
       <c r="K116" s="47"/>
       <c r="L116" s="47"/>
       <c r="M116" s="47"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17">
       <c r="A117" s="19" t="s">
         <v>36</v>
       </c>
@@ -4540,71 +4548,71 @@
       <c r="L117" s="47"/>
       <c r="M117" s="47"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17">
       <c r="A118" t="s">
         <v>105</v>
       </c>
       <c r="B118" s="37">
         <f ca="1">SUM(B106:B109)</f>
-        <v>338.36</v>
+        <v>852.40785714285744</v>
       </c>
       <c r="F118" s="47"/>
       <c r="K118" s="47"/>
       <c r="L118" s="47"/>
       <c r="M118" s="47"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17">
       <c r="A119" t="s">
         <v>106</v>
       </c>
       <c r="B119" s="38">
         <f ca="1">SUM(B110:B113)</f>
-        <v>240</v>
+        <v>796.62714285714287</v>
       </c>
       <c r="F119" s="47"/>
       <c r="K119" s="47"/>
       <c r="L119" s="47"/>
       <c r="M119" s="47"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17">
       <c r="B120" s="37">
         <f ca="1">SUM(B118:B119)</f>
-        <v>578.36</v>
+        <v>1649.0350000000003</v>
       </c>
       <c r="F120" s="47"/>
       <c r="K120" s="47"/>
       <c r="L120" s="47"/>
       <c r="M120" s="47"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17">
       <c r="B121" s="13"/>
       <c r="F121" s="47"/>
       <c r="K121" s="47"/>
       <c r="L121" s="47"/>
       <c r="M121" s="47"/>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17">
       <c r="B122" s="13"/>
       <c r="F122" s="47"/>
       <c r="K122" s="47"/>
       <c r="L122" s="47"/>
       <c r="M122" s="47"/>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17">
       <c r="B123" s="13"/>
       <c r="F123" s="47"/>
       <c r="K123" s="47"/>
       <c r="L123" s="47"/>
       <c r="M123" s="47"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17">
       <c r="B124" s="13"/>
       <c r="F124" s="47"/>
       <c r="K124" s="47"/>
       <c r="L124" s="47"/>
       <c r="M124" s="47"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17">
       <c r="B125" s="15"/>
       <c r="F125" s="47"/>
       <c r="K125" s="49"/>
@@ -4612,19 +4620,19 @@
       <c r="M125" s="49"/>
       <c r="N125" s="18"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17">
       <c r="F126" s="47"/>
       <c r="K126" s="47"/>
       <c r="L126" s="47"/>
       <c r="M126" s="47"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17">
       <c r="F127" s="47"/>
       <c r="K127" s="47"/>
       <c r="L127" s="47"/>
       <c r="M127" s="47"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17">
       <c r="F128" s="47"/>
       <c r="G128" s="47"/>
       <c r="H128" s="46"/>
@@ -4634,10 +4642,10 @@
       <c r="L128" s="47"/>
       <c r="M128" s="47"/>
     </row>
-    <row r="129" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="8:13">
       <c r="H129" s="12"/>
     </row>
-    <row r="131" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="8:13">
       <c r="H131" s="40"/>
       <c r="M131" s="22"/>
     </row>
@@ -4657,7 +4665,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4665,28 +4678,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B17" sqref="B17:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="13" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
@@ -4701,7 +4714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4715,7 +4728,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>89</v>
       </c>
@@ -4727,7 +4740,7 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="E4" t="s">
         <v>55</v>
       </c>
@@ -4742,7 +4755,7 @@
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -4763,7 +4776,7 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" s="28" t="s">
         <v>57</v>
       </c>
@@ -4782,7 +4795,7 @@
       <c r="M6" s="80"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" s="28" t="s">
         <v>58</v>
       </c>
@@ -4801,7 +4814,7 @@
       <c r="M7" s="80"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="21" customFormat="1">
       <c r="A8" s="57"/>
       <c r="B8"/>
       <c r="D8" s="47"/>
@@ -4815,7 +4828,7 @@
       <c r="L8" s="80"/>
       <c r="M8" s="80"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -4831,7 +4844,7 @@
       <c r="M9" s="47"/>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4850,7 +4863,7 @@
       <c r="M10" s="47"/>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14">
       <c r="D11" s="47"/>
       <c r="E11" s="47"/>
       <c r="F11" s="47"/>
@@ -4863,7 +4876,7 @@
       <c r="M11" s="47"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14">
       <c r="D12" s="47"/>
       <c r="E12" s="47"/>
       <c r="F12" s="78"/>
@@ -4876,7 +4889,7 @@
       <c r="M12" s="47"/>
       <c r="N12" s="21"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14">
       <c r="D13" s="47"/>
       <c r="E13" s="47"/>
       <c r="F13" s="47"/>
@@ -4889,7 +4902,7 @@
       <c r="M13" s="47"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -4900,7 +4913,7 @@
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -4909,7 +4922,7 @@
       <c r="G15" s="21"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -4918,7 +4931,7 @@
       <c r="G16" s="21"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14">
       <c r="B17" s="91" t="s">
         <v>20</v>
       </c>
@@ -4929,7 +4942,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -4948,7 +4961,7 @@
       <c r="H18" s="92"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -4968,7 +4981,7 @@
       <c r="H19" s="66"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4988,7 +5001,7 @@
       <c r="H20" s="66"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -5008,7 +5021,7 @@
       <c r="H21" s="66"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15">
       <c r="B22" s="27">
         <f>C21</f>
         <v>200000</v>
@@ -5023,7 +5036,7 @@
       <c r="H22" s="66"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14">
       <c r="B23" s="21"/>
       <c r="C23" s="91"/>
       <c r="D23" s="21"/>
@@ -5032,7 +5045,7 @@
       <c r="G23" s="21"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -5046,13 +5059,13 @@
       <c r="G24" s="52"/>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14">
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -5061,7 +5074,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14">
       <c r="A27" s="10" t="s">
         <v>90</v>
       </c>
@@ -5078,7 +5091,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="70"/>
     </row>
-    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -5097,7 +5110,7 @@
       <c r="J28" s="66"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -5120,7 +5133,7 @@
       <c r="K29" s="53"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -5144,7 +5157,7 @@
       <c r="L30" s="13"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -5168,7 +5181,7 @@
       <c r="L31" s="13"/>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15">
       <c r="B32" s="27">
         <f>C31</f>
         <v>300000</v>
@@ -5186,7 +5199,7 @@
       <c r="K32" s="52"/>
       <c r="L32" s="13"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17">
       <c r="B33" s="21"/>
       <c r="C33" s="91"/>
       <c r="D33" s="21"/>
@@ -5199,7 +5212,7 @@
       <c r="K33" s="20"/>
       <c r="L33" s="26"/>
     </row>
-    <row r="34" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -5214,7 +5227,7 @@
       <c r="K34" s="20"/>
       <c r="L34" s="26"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" t="s">
@@ -5227,7 +5240,7 @@
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17">
       <c r="B36" s="37"/>
       <c r="C36" s="4"/>
       <c r="I36" s="47"/>
@@ -5235,7 +5248,7 @@
       <c r="K36" s="21"/>
       <c r="Q36" s="18"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -5246,7 +5259,7 @@
       <c r="K37" s="21"/>
       <c r="Q37" s="18"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17">
       <c r="B38" s="37"/>
       <c r="C38" s="4"/>
       <c r="I38" s="47"/>
@@ -5254,7 +5267,7 @@
       <c r="K38" s="21"/>
       <c r="Q38" s="18"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17">
       <c r="A39" s="19" t="s">
         <v>51</v>
       </c>
@@ -5266,7 +5279,7 @@
       <c r="K39" s="21"/>
       <c r="Q39" s="18"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -5295,7 +5308,7 @@
       <c r="K40" s="21"/>
       <c r="Q40" s="18"/>
     </row>
-    <row r="41" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -5334,7 +5347,7 @@
       <c r="K41" s="21"/>
       <c r="Q41" s="18"/>
     </row>
-    <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -5373,7 +5386,7 @@
       <c r="K42" s="21"/>
       <c r="Q42" s="18"/>
     </row>
-    <row r="43" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -5412,7 +5425,7 @@
       <c r="K43" s="21"/>
       <c r="Q43" s="18"/>
     </row>
-    <row r="44" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -5453,7 +5466,7 @@
       <c r="K44" s="21"/>
       <c r="Q44" s="18"/>
     </row>
-    <row r="45" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -5487,7 +5500,7 @@
       <c r="K45" s="21"/>
       <c r="Q45" s="18"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17">
       <c r="B46" s="37"/>
       <c r="C46" s="4"/>
       <c r="E46" s="13"/>
@@ -5502,7 +5515,7 @@
       <c r="K46" s="21"/>
       <c r="Q46" s="18"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -5531,7 +5544,7 @@
       <c r="K47" s="21"/>
       <c r="Q47" s="18"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>73</v>
       </c>
@@ -5549,7 +5562,7 @@
       <c r="K48" s="21"/>
       <c r="Q48" s="18"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -5564,7 +5577,7 @@
       <c r="K49" s="21"/>
       <c r="Q49" s="18"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -5582,7 +5595,7 @@
       <c r="K50" s="21"/>
       <c r="Q50" s="18"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -5598,7 +5611,7 @@
       <c r="K51" s="21"/>
       <c r="Q51" s="18"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17">
       <c r="B52" s="37"/>
       <c r="C52" s="4"/>
       <c r="I52" s="47"/>
@@ -5606,7 +5619,7 @@
       <c r="K52" s="21"/>
       <c r="Q52" s="18"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -5620,7 +5633,7 @@
       <c r="K53" s="21"/>
       <c r="Q53" s="18"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17">
       <c r="B54" s="37"/>
       <c r="C54" s="4"/>
       <c r="I54" s="47"/>
@@ -5628,7 +5641,7 @@
       <c r="K54" s="21"/>
       <c r="Q54" s="18"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -5642,7 +5655,7 @@
       <c r="K55" s="21"/>
       <c r="Q55" s="18"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17">
       <c r="B56" s="37"/>
       <c r="C56" s="4"/>
       <c r="E56" s="65"/>
@@ -5654,7 +5667,7 @@
       <c r="K56" s="21"/>
       <c r="Q56" s="18"/>
     </row>
-    <row r="57" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="15">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -5673,7 +5686,7 @@
       <c r="K57" s="21"/>
       <c r="Q57" s="18"/>
     </row>
-    <row r="58" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="15">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -5692,7 +5705,7 @@
       <c r="K58" s="21"/>
       <c r="Q58" s="18"/>
     </row>
-    <row r="59" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="15">
       <c r="B59" s="37"/>
       <c r="C59" s="4"/>
       <c r="E59" s="5"/>
@@ -5703,7 +5716,7 @@
       <c r="K59" s="21"/>
       <c r="Q59" s="18"/>
     </row>
-    <row r="60" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="15">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -5722,7 +5735,7 @@
       <c r="K60" s="21"/>
       <c r="Q60" s="18"/>
     </row>
-    <row r="61" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="15">
       <c r="B61" s="62"/>
       <c r="C61" s="4"/>
       <c r="E61" s="5"/>
@@ -5734,7 +5747,7 @@
       <c r="K61" s="21"/>
       <c r="Q61" s="18"/>
     </row>
-    <row r="62" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="15">
       <c r="B62" s="62"/>
       <c r="C62" s="4"/>
       <c r="E62" s="13"/>
@@ -5746,7 +5759,7 @@
       <c r="K62" s="21"/>
       <c r="Q62" s="18"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17">
       <c r="A63" s="19" t="s">
         <v>67</v>
       </c>
@@ -5759,7 +5772,7 @@
       <c r="L63" s="19"/>
       <c r="Q63" s="18"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -5786,7 +5799,7 @@
       <c r="K64" s="53"/>
       <c r="Q64" s="18"/>
     </row>
-    <row r="65" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="15">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -5823,7 +5836,7 @@
       <c r="K65" s="21"/>
       <c r="Q65" s="18"/>
     </row>
-    <row r="66" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="15">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -5862,7 +5875,7 @@
       <c r="K66" s="21"/>
       <c r="Q66" s="18"/>
     </row>
-    <row r="67" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="15">
       <c r="B67" s="37"/>
       <c r="C67" s="4"/>
       <c r="D67" t="s">
@@ -5895,7 +5908,7 @@
       <c r="K67" s="21"/>
       <c r="Q67" s="18"/>
     </row>
-    <row r="68" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="15">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -5934,7 +5947,7 @@
       <c r="K68" s="21"/>
       <c r="Q68" s="18"/>
     </row>
-    <row r="69" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="15">
       <c r="B69" s="37"/>
       <c r="C69" s="4"/>
       <c r="E69" s="5">
@@ -5960,7 +5973,7 @@
       <c r="K69" s="21"/>
       <c r="Q69" s="18"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -5983,7 +5996,7 @@
       <c r="K70" s="21"/>
       <c r="Q70" s="18"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17">
       <c r="B71" s="37"/>
       <c r="C71" s="60"/>
       <c r="E71" s="13"/>
@@ -6006,7 +6019,7 @@
       <c r="K71" s="21"/>
       <c r="Q71" s="18"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>65</v>
       </c>
@@ -6025,7 +6038,7 @@
       </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -6041,7 +6054,7 @@
       <c r="J73" s="49"/>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17">
       <c r="B74" s="37">
         <f ca="1">SUM(B72:B73)</f>
         <v>0</v>
@@ -6055,7 +6068,7 @@
       <c r="J74" s="12"/>
       <c r="K74" s="21"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17">
       <c r="B75" s="37"/>
       <c r="C75" s="4"/>
       <c r="H75" s="18"/>
@@ -6064,7 +6077,7 @@
       <c r="K75" s="52"/>
       <c r="L75" s="16"/>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>69</v>
       </c>
@@ -6080,7 +6093,7 @@
       <c r="K76" s="52"/>
       <c r="L76" s="16"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17">
       <c r="B77" s="37"/>
       <c r="C77" s="4"/>
       <c r="I77" s="47"/>
@@ -6088,7 +6101,7 @@
       <c r="K77" s="52"/>
       <c r="L77" s="16"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -6106,7 +6119,7 @@
       <c r="K78" s="52"/>
       <c r="L78" s="16"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17">
       <c r="B79" s="37"/>
       <c r="C79" s="4"/>
       <c r="G79" s="18"/>
@@ -6116,7 +6129,7 @@
       <c r="K79" s="52"/>
       <c r="L79" s="16"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17">
       <c r="A80" s="2" t="s">
         <v>12</v>
       </c>
@@ -6127,7 +6140,7 @@
       <c r="K80" s="48"/>
       <c r="L80" s="16"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17">
       <c r="B81" s="11"/>
       <c r="C81" t="s">
         <v>13</v>
@@ -6139,7 +6152,7 @@
       <c r="K81" s="48"/>
       <c r="L81" s="16"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17">
       <c r="B82" s="37"/>
       <c r="C82" s="4"/>
       <c r="H82" s="46"/>
@@ -6148,7 +6161,7 @@
       <c r="K82" s="47"/>
       <c r="L82" s="16"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -6166,7 +6179,7 @@
       <c r="K83" s="47"/>
       <c r="L83" s="13"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17">
       <c r="B84" s="37">
         <f>-IF(B14&gt;=B24,0,IF(B14&lt;B24,IF((B14+B5+B44)&gt;B24,(B24-B14)*D18,((B5+B44)*D18))))</f>
         <v>0</v>
@@ -6181,7 +6194,7 @@
       <c r="K84" s="48"/>
       <c r="L84" s="16"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17">
       <c r="B85" s="37">
         <f ca="1">IF(B60=0,0,-MIN(B60,SUM(B83:B84)))</f>
         <v>-200</v>
@@ -6196,7 +6209,7 @@
       <c r="K85" s="52"/>
       <c r="L85" s="16"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17">
       <c r="B86" s="37">
         <f ca="1">IF(AND((B5+B44+B14)&gt;=B28,(B5+B44+B14)&lt;=C28),(B5+B44)*D28,IF(AND((B5+B44+B14)&gt;B29,(B5+B44+B14)&lt;=C29),IF((B5+B44+B14-B29)&gt;(B5+B44),(B5+B44)*D29,((B5+B44+B14-B29)*D29)+((B5+B44-(B5+B44+B14-B29))*D28)),IF(AND((B5+B44+B14)&gt;B30,(B5+B44+B14)&lt;=C30),IF((B5+B44+B14-B30)&gt;(B5+B44),(B5+B44)*D30,IF((B5+B44+B14-B29)&gt;(B5+B44),(((B5+B44+B14-B30)*D30)+((B5+B44-(B5+B44+B14-B30))*D29)),((B5+B44+B14-B30)*D30)+((C29-B29)*D29)+((B5+B44-(B5+B44+B14-B29))*D28))),IF(AND((B5+B44+B14)&gt;B31,(B5+B44+B14)&lt;=C31),IF((B5+B44+B14-B31)&gt;(B5+B44),(B5+B44)*D31,IF((B5+B44+B14-B30)&gt;(B5+B44),(((B5+B44+B14-B31)*D31)+((B5+B44-(B5+B44+B14-B31))*D30)),IF((B5+B44+B14-B29)&gt;(B5+B44),(((B5+B44+B14-B31)*D31)+((C30-B30)*D30)+((B5+B44-(B5+B44+B14-B30))*D29)),((B5+B44+B14-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B5+B44-(B5+B44+B14-B29))*D28)))),IF((B5+B44+B14)&gt;B32,IF((B5+B44+B14-B32)&gt;(B5+B44),(B5+B44)*D32,IF((B5+B44+B14-B31)&gt;(B5+B44),(((B5+B44+B14-B32)*D32)+((B5+B44-(B5+B44+B14-B32))*D31)),IF((B5+B44+B14-B30)&gt;(B5+B44),(((B5+B44+B14-B32)*D32)+((C31-B31)*D31)+((B5+B44-(B5+B44+B14-B31))*D30)),IF((B5+B44+B14-B29)&gt;(B5+B44),(((B5+B44+B14-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((B5+B44-(B5+B44+B14-B30))*D29)),((B5+B44+B14-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B5+B44-(B5+B44+B14-B29))*D28))))))))))</f>
         <v>240</v>
@@ -6210,7 +6223,7 @@
       <c r="J86" s="53"/>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17">
       <c r="B87" s="37">
         <f>-IF(B14&gt;=B34,0,IF(B14&lt;B34,IF((B14+B5+B44)&gt;B34,(B34-B14)*D28,((B5+B44)*D28))))</f>
         <v>0</v>
@@ -6225,7 +6238,7 @@
       <c r="K87" s="52"/>
       <c r="L87" s="13"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17">
       <c r="B88" s="38">
         <f ca="1">IF(B76=0,0,-MIN(B76,SUM(B86,B87)))</f>
         <v>0</v>
@@ -6240,7 +6253,7 @@
       <c r="K88" s="21"/>
       <c r="L88" s="13"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17">
       <c r="A89" s="10" t="s">
         <v>21</v>
       </c>
@@ -6255,7 +6268,7 @@
       <c r="L89" s="48"/>
       <c r="M89" s="47"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17">
       <c r="E90" s="18"/>
       <c r="F90" s="49"/>
       <c r="K90" s="47"/>
@@ -6263,14 +6276,14 @@
       <c r="M90" s="47"/>
       <c r="Q90" s="15"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17">
       <c r="B91" s="13"/>
       <c r="F91" s="47"/>
       <c r="K91" s="47"/>
       <c r="L91" s="47"/>
       <c r="M91" s="47"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17">
       <c r="A92" s="19" t="s">
         <v>36</v>
       </c>
@@ -6280,7 +6293,7 @@
       <c r="L92" s="47"/>
       <c r="M92" s="47"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>105</v>
       </c>
@@ -6293,7 +6306,7 @@
       <c r="L93" s="47"/>
       <c r="M93" s="47"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -6306,7 +6319,7 @@
       <c r="L94" s="47"/>
       <c r="M94" s="47"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17">
       <c r="B95" s="37">
         <f ca="1">SUM(B93:B94)</f>
         <v>578.36</v>
@@ -6316,35 +6329,35 @@
       <c r="L95" s="47"/>
       <c r="M95" s="47"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17">
       <c r="B96" s="13"/>
       <c r="F96" s="47"/>
       <c r="K96" s="47"/>
       <c r="L96" s="47"/>
       <c r="M96" s="47"/>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:14">
       <c r="B97" s="13"/>
       <c r="F97" s="47"/>
       <c r="K97" s="47"/>
       <c r="L97" s="47"/>
       <c r="M97" s="47"/>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:14">
       <c r="B98" s="13"/>
       <c r="F98" s="47"/>
       <c r="K98" s="47"/>
       <c r="L98" s="47"/>
       <c r="M98" s="47"/>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:14">
       <c r="B99" s="13"/>
       <c r="F99" s="47"/>
       <c r="K99" s="47"/>
       <c r="L99" s="47"/>
       <c r="M99" s="47"/>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:14">
       <c r="B100" s="15"/>
       <c r="F100" s="47"/>
       <c r="K100" s="49"/>
@@ -6352,19 +6365,19 @@
       <c r="M100" s="49"/>
       <c r="N100" s="18"/>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:14">
       <c r="F101" s="47"/>
       <c r="K101" s="47"/>
       <c r="L101" s="47"/>
       <c r="M101" s="47"/>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:14">
       <c r="F102" s="47"/>
       <c r="K102" s="47"/>
       <c r="L102" s="47"/>
       <c r="M102" s="47"/>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:14">
       <c r="F103" s="47"/>
       <c r="G103" s="47"/>
       <c r="H103" s="46"/>
@@ -6374,10 +6387,10 @@
       <c r="L103" s="47"/>
       <c r="M103" s="47"/>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:14">
       <c r="H104" s="12"/>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:14">
       <c r="H106" s="40"/>
       <c r="M106" s="22"/>
     </row>
@@ -6391,7 +6404,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6399,34 +6417,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="13" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6443,7 +6461,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="3" t="s">
         <v>95</v>
       </c>
@@ -6460,7 +6478,7 @@
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -6480,7 +6498,7 @@
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="12"/>
@@ -6494,7 +6512,7 @@
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -6508,7 +6526,7 @@
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -6525,7 +6543,7 @@
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6545,7 +6563,7 @@
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -6559,7 +6577,7 @@
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="E10" s="21"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
@@ -6573,7 +6591,7 @@
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -6587,7 +6605,7 @@
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -6595,12 +6613,12 @@
         <v>139000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -6609,7 +6627,7 @@
       <c r="G16" s="21"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14">
       <c r="B17" s="91" t="s">
         <v>20</v>
       </c>
@@ -6620,7 +6638,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -6644,7 +6662,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -6669,7 +6687,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -6694,7 +6712,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -6719,7 +6737,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15">
       <c r="B22" s="27">
         <f>C21</f>
         <v>200000</v>
@@ -6738,7 +6756,7 @@
       <c r="L22" s="5"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14">
       <c r="B23" s="21"/>
       <c r="C23" s="91"/>
       <c r="D23" s="21"/>
@@ -6747,7 +6765,7 @@
       <c r="G23" s="21"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -6761,14 +6779,14 @@
       <c r="G24" s="52"/>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14">
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="12"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -6777,7 +6795,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14">
       <c r="A27" s="10" t="s">
         <v>90</v>
       </c>
@@ -6794,7 +6812,7 @@
       <c r="J27" s="10"/>
       <c r="K27" s="25"/>
     </row>
-    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -6812,7 +6830,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -6835,7 +6853,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -6859,7 +6877,7 @@
       <c r="L30" s="13"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -6883,7 +6901,7 @@
       <c r="L31" s="13"/>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15">
       <c r="B32" s="27">
         <f>C31</f>
         <v>300000</v>
@@ -6901,7 +6919,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="13"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="B33" s="21"/>
       <c r="C33" s="91"/>
       <c r="D33" s="21"/>
@@ -6914,7 +6932,7 @@
       <c r="K33" s="16"/>
       <c r="L33" s="26"/>
     </row>
-    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -6929,7 +6947,7 @@
       <c r="K34" s="16"/>
       <c r="L34" s="26"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" t="s">
@@ -6939,19 +6957,19 @@
       <c r="F35" s="44"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="28" t="s">
         <v>98</v>
       </c>
@@ -6960,7 +6978,7 @@
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" s="28" t="s">
         <v>99</v>
       </c>
@@ -6969,12 +6987,12 @@
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="28">
       <c r="A41" s="84" t="s">
         <v>100</v>
       </c>
@@ -6984,7 +7002,7 @@
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="28">
       <c r="A42" s="84" t="s">
         <v>101</v>
       </c>
@@ -6994,7 +7012,7 @@
       </c>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="28" t="s">
         <v>102</v>
       </c>
@@ -7004,14 +7022,14 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="E44" s="13"/>
       <c r="F44" s="44"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -7021,7 +7039,7 @@
       <c r="H45" s="4"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="B46" s="11"/>
       <c r="C46" t="s">
         <v>13</v>
@@ -7031,14 +7049,14 @@
       <c r="K46" s="4"/>
       <c r="L46" s="16"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="H47" s="36"/>
       <c r="I47" s="18"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="16"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -7053,7 +7071,7 @@
       <c r="K48" s="4"/>
       <c r="L48" s="16"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17">
       <c r="B49" s="37">
         <f>-IF(B12&gt;=B24,0,IF(B12&lt;B24,IF((B12+B4-B43)&gt;B24,(B24-B12)*D18,(B4-B43)*D18)))</f>
         <v>0</v>
@@ -7065,7 +7083,7 @@
       <c r="K49" s="4"/>
       <c r="L49" s="16"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17">
       <c r="B50" s="12">
         <f>IF(AND((B4-B43+B12)&gt;=B28,(B4-B43+B12)&lt;=C28),(B4-B43)*D28,IF(AND((B4-B43+B12)&gt;B29,(B4-B43+B12)&lt;=C29),IF((B4-B43+B12-B29)&gt;(B4-B43),(B4-B43)*D29,((B4-B43+B12-B29)*D29)+((B4-B43-(B4-B43+B12-B29))*D28)),IF(AND((B4-B43+B12)&gt;B30,(B4-B43+B12)&lt;=C30),IF((B4-B43+B12-B30)&gt;(B4-B43),(B4-B43)*D30,IF((B4-B43+B12-B29)&gt;(B4-B43),(((B4-B43+B12-B30)*D30)+((B4-B43-(B4-B43+B12-B30))*D29)),((B4-B43+B12-B30)*D30)+((C29-B29)*D29)+((B4-B43-(B4-B43+B12-B29))*D28))),IF(AND((B4-B43+B12)&gt;B31,(B4-B43+B12)&lt;=C31),IF((B4-B43+B12-B31)&gt;(B4-B43),(B4-B43)*D31,IF((B4-B43+B12-B30)&gt;(B4-B43),(((B4-B43+B12-B31)*D31)+((B4-B43-(B4-B43+B12-B31))*D30)),IF((B4-B43+B12-B29)&gt;(B4-B43),(((B4-B43+B12-B31)*D31)+((C30-B30)*D30)+((B4-B43-(B4-B43+B12-B30))*D29)),((B4-B43+B12-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B4-B43-(B4-B43+B12-B29))*D28)))),IF((B4-B43+B12)&gt;B32,IF((B4-B43+B12-B32)&gt;(B4-B43),(B4-B43)*D32,IF((B4-B43+B12-B31)&gt;(B4-B43),(((B4-B43+B12-B32)*D32)+((B4-B43-(B4-B43+B12-B32))*D31)),IF((B4-B43+B12-B30)&gt;(B4-B43),(((B4-B43+B12-B32)*D32)+((C31-B31)*D31)+((B4-B43-(B4-B43+B12-B31))*D30)),IF((B4-B43+B12-B29)&gt;(B4-B43),(((B4-B43+B12-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((B4-B43-(B4-B43+B12-B30))*D29)),((B4-B43+B12-B32)*D32)+((C31-B31)*D31)+((C30-B30)*D30)+((C29-B29)*D29)+((B4-B43-(B4-B43+B12-B29))*D28))))))))))</f>
         <v>102</v>
@@ -7074,7 +7092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17">
       <c r="B51" s="39">
         <f>-IF(B12&gt;=B34,0,IF(B12&lt;B34,IF((B12+B4-B43)&gt;B34,(B34-B12)*D28,(B4-B43)*D28)))</f>
         <v>0</v>
@@ -7083,7 +7101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17">
       <c r="B52" s="86">
         <f>B43</f>
         <v>150</v>
@@ -7092,7 +7110,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17">
       <c r="A53" s="10" t="s">
         <v>21</v>
       </c>
@@ -7109,7 +7127,7 @@
       <c r="L53" s="48"/>
       <c r="M53" s="47"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17">
       <c r="E54" s="18"/>
       <c r="F54" s="49"/>
       <c r="G54" s="47"/>
@@ -7121,7 +7139,7 @@
       <c r="M54" s="47"/>
       <c r="Q54" s="15"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17">
       <c r="B55" s="13"/>
       <c r="F55" s="47"/>
       <c r="G55" s="47"/>
@@ -7132,7 +7150,7 @@
       <c r="L55" s="47"/>
       <c r="M55" s="47"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17">
       <c r="A56" s="19" t="s">
         <v>36</v>
       </c>
@@ -7146,7 +7164,7 @@
       <c r="L56" s="47"/>
       <c r="M56" s="47"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>105</v>
       </c>
@@ -7163,7 +7181,7 @@
       <c r="L57" s="47"/>
       <c r="M57" s="47"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -7180,7 +7198,7 @@
       <c r="L58" s="47"/>
       <c r="M58" s="47"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17">
       <c r="A59" s="89" t="s">
         <v>97</v>
       </c>
@@ -7197,7 +7215,7 @@
       <c r="L59" s="47"/>
       <c r="M59" s="47"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17">
       <c r="B60" s="13">
         <f>SUM(B57:B59)</f>
         <v>473</v>
@@ -7211,7 +7229,7 @@
       <c r="L60" s="47"/>
       <c r="M60" s="47"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17">
       <c r="B61" s="13"/>
       <c r="F61" s="47"/>
       <c r="G61" s="47"/>
@@ -7222,7 +7240,7 @@
       <c r="L61" s="47"/>
       <c r="M61" s="47"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17">
       <c r="B62" s="13"/>
       <c r="F62" s="47"/>
       <c r="G62" s="47"/>
@@ -7233,7 +7251,7 @@
       <c r="L62" s="47"/>
       <c r="M62" s="47"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17">
       <c r="B63" s="13"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47"/>
@@ -7244,7 +7262,7 @@
       <c r="L63" s="47"/>
       <c r="M63" s="47"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17">
       <c r="B64" s="13"/>
       <c r="F64" s="47"/>
       <c r="G64" s="47"/>
@@ -7255,7 +7273,7 @@
       <c r="L64" s="47"/>
       <c r="M64" s="47"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:13">
       <c r="B65" s="15"/>
       <c r="F65" s="47"/>
       <c r="G65" s="47"/>
@@ -7266,7 +7284,7 @@
       <c r="L65" s="47"/>
       <c r="M65" s="47"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:13">
       <c r="F66" s="47"/>
       <c r="G66" s="47"/>
       <c r="H66" s="46"/>
@@ -7276,7 +7294,7 @@
       <c r="L66" s="47"/>
       <c r="M66" s="47"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:13">
       <c r="F67" s="47"/>
       <c r="G67" s="47"/>
       <c r="H67" s="46"/>
@@ -7286,7 +7304,7 @@
       <c r="L67" s="47"/>
       <c r="M67" s="47"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:13">
       <c r="F68" s="47"/>
       <c r="G68" s="47"/>
       <c r="H68" s="46"/>
@@ -7296,15 +7314,20 @@
       <c r="L68" s="47"/>
       <c r="M68" s="47"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:13">
       <c r="H69" s="12"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:13">
       <c r="H71" s="40"/>
       <c r="M71" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>